<commit_message>
Corrected the DataSet value for dsp feeder map
</commit_message>
<xml_diff>
--- a/AutoFirmwareUpgrade/CashelFirmwareAutomatedTest/TestDataFiles/CablingDataSet/3U3I3I3I3I.xlsx
+++ b/AutoFirmwareUpgrade/CashelFirmwareAutomatedTest/TestDataFiles/CablingDataSet/3U3I3I3I3I.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{776E52E5-571A-45AD-BF1A-DF6E8FB4639E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0099B473-FA76-4404-870A-A66A1E50A734}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DeviceInfo" sheetId="3" r:id="rId1"/>
@@ -1574,8 +1574,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1609,7 +1609,7 @@
         <v>126</v>
       </c>
       <c r="B4" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1617,7 +1617,7 @@
         <v>127</v>
       </c>
       <c r="B5" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1625,7 +1625,7 @@
         <v>128</v>
       </c>
       <c r="B6" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1646,7 +1646,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>

</xml_diff>